<commit_message>
add: first requirement changes
</commit_message>
<xml_diff>
--- a/TestCase_Results_WordCount_Mohit_smw572.xlsx
+++ b/TestCase_Results_WordCount_Mohit_smw572.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c271e4f1ba4d609/Desktop/UTSA/SE/Mohit_sharma/CS-5103_smw572_mohitsharma/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\UTSA\SE\Mohit_sharma\CS-5103_smw572_mohitsharma\CS-5103_smw572_mohitsharma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{632E7ECB-09B9-4E88-84C0-46553EE392FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE749716-1621-414B-BFF8-B48E88A59421}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE8421A-489B-4AA3-9E00-15975097E200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{13E32D60-6303-4965-8B3C-2C1ED618534E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
   <si>
     <t>The string with one word must give one word as output in list</t>
   </si>
@@ -59,9 +59,6 @@
     <t>String with alphanumeric words  are considered as unique words such as  abc123 6abc789</t>
   </si>
   <si>
-    <t>Testcase#</t>
-  </si>
-  <si>
     <t>Gives an empty list as in output</t>
   </si>
   <si>
@@ -80,30 +77,6 @@
     <t>Get all words added into the list  in output</t>
   </si>
   <si>
-    <t>4.a</t>
-  </si>
-  <si>
-    <t>4.b</t>
-  </si>
-  <si>
-    <t>4.c</t>
-  </si>
-  <si>
-    <t>4.d</t>
-  </si>
-  <si>
-    <t>4.e</t>
-  </si>
-  <si>
-    <t>4.f</t>
-  </si>
-  <si>
-    <t>4.g</t>
-  </si>
-  <si>
-    <t>4.h</t>
-  </si>
-  <si>
     <t xml:space="preserve">Requirement number in requirement document </t>
   </si>
   <si>
@@ -132,13 +105,143 @@
   </si>
   <si>
     <t>Empty_string_should_give_empty_list_with_no_words</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>4.1.3</t>
+  </si>
+  <si>
+    <t>4.1.4</t>
+  </si>
+  <si>
+    <t>4.1.5</t>
+  </si>
+  <si>
+    <t>4.1.6</t>
+  </si>
+  <si>
+    <t>4.1.7</t>
+  </si>
+  <si>
+    <t>4.1.8</t>
+  </si>
+  <si>
+    <t>Functionality</t>
+  </si>
+  <si>
+    <t>Distinct WordCount</t>
+  </si>
+  <si>
+    <t>4.2.1</t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>4.2.3</t>
+  </si>
+  <si>
+    <t>4.2.4</t>
+  </si>
+  <si>
+    <t>4.2.5</t>
+  </si>
+  <si>
+    <t>4.2.6</t>
+  </si>
+  <si>
+    <t>4.2.7</t>
+  </si>
+  <si>
+    <t>4.2.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The empty string should give character count as 0. </t>
+  </si>
+  <si>
+    <t>An empty String should give the total number of spaces in the String/file.</t>
+  </si>
+  <si>
+    <t>The string with only one period (‘.’) should give correct output also.</t>
+  </si>
+  <si>
+    <t>Alphanumeric words, Special characters  and Numbers are also to be considered as characters.</t>
+  </si>
+  <si>
+    <t>If there are multiple spaces in between two words, then the character count should be given counting all the characters.</t>
+  </si>
+  <si>
+    <t>The string with multiple lines should count a newline character as a character and give correct character count.</t>
+  </si>
+  <si>
+    <t>This program should be capable of counting the characters in the large strings too.</t>
+  </si>
+  <si>
+    <t>The string with one word must give the count of characters in that word.</t>
+  </si>
+  <si>
+    <t>Leading spaces in the lines should also be counted in the total characters in the string.</t>
+  </si>
+  <si>
+    <t>4.2.9</t>
+  </si>
+  <si>
+    <t>4.2.10</t>
+  </si>
+  <si>
+    <t>NumberOfChar: 0
+NumberOfLines:0</t>
+  </si>
+  <si>
+    <t>NumberOfChar: 5
+NumberOfLines:1</t>
+  </si>
+  <si>
+    <t>If String is having only one new line character(/n) in it.</t>
+  </si>
+  <si>
+    <t>NumberOfChar: 21
+NumberOfLines:1</t>
+  </si>
+  <si>
+    <t>NumberOfChar: 1
+NumberOfLines:1</t>
+  </si>
+  <si>
+    <t>NumberOfChar: 24
+NumberOfLines:4</t>
+  </si>
+  <si>
+    <t>NumberOfChar: 47
+NumberOfLines:1</t>
+  </si>
+  <si>
+    <t>NumberOfChar: 869
+NumberOfLines:16</t>
+  </si>
+  <si>
+    <t>NumberOfChar: 79948
+NumberOfLines:1381</t>
+  </si>
+  <si>
+    <t>NumberOfChar: 38
+NumberOfLines:2</t>
+  </si>
+  <si>
+    <t>CharacterCount
+and Line count scenarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +272,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -189,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -252,7 +361,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -270,7 +379,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -285,13 +394,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -303,12 +412,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -318,9 +423,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -331,6 +434,34 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -346,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -355,43 +486,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -709,227 +862,430 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C70BAD-E71C-4C1A-9055-85AD7A7430AE}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="88.28515625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="88.28515625" style="17" customWidth="1"/>
     <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" style="20" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="17" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" customWidth="1"/>
     <col min="7" max="7" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19"/>
+      <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19"/>
+      <c r="B5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="16" t="s">
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
+      <c r="B9" s="26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="C9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
-        <v>8</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>30</v>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
+      <c r="B19" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A19"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>